<commit_message>
thêm số đt tài xế
</commit_message>
<xml_diff>
--- a/compass_app/docs/Thông tin xe.xlsx
+++ b/compass_app/docs/Thông tin xe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\flutter_samples\compass_app\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D729F9AB-5FD2-46F9-89F1-D364A9D613B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBAB47F0-AEDD-47AB-B475-B9026DE5881F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{3C428B59-A54A-4BFD-A7E0-50364FCFE182}"/>
   </bookViews>
@@ -16,28 +16,17 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Thông tin xe</t>
   </si>
@@ -146,6 +135,9 @@
   </si>
   <si>
     <t>tải trọng m3 luôn dùng cho xe bồn nên ko tạo cột này nữa</t>
+  </si>
+  <si>
+    <t>sdttaixe</t>
   </si>
 </sst>
 </file>
@@ -516,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05172157-2725-4999-B7F1-ECF5E7BDA8FD}">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.4"/>
@@ -594,7 +586,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="90" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="36" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>7</v>
       </c>
@@ -772,6 +764,14 @@
       </c>
       <c r="B32" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>12</v>
+      </c>
+      <c r="B34" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>